<commit_message>
Added the photometric P profile for comparison.
</commit_message>
<xml_diff>
--- a/index/data/pw_P_photometric.xlsx
+++ b/index/data/pw_P_photometric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7446CC-D9B2-4A96-9D9D-BA5115C45882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD42BCF-164D-4237-96FB-AD20694F7652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="117">
   <si>
     <t>Sample</t>
   </si>
@@ -48,333 +48,12 @@
     <t>A</t>
   </si>
   <si>
-    <t>A bw</t>
-  </si>
-  <si>
-    <t>BL-A1.1-0</t>
-  </si>
-  <si>
-    <t>BL-A1.1-1</t>
-  </si>
-  <si>
-    <t>BL-A1.1-2</t>
-  </si>
-  <si>
-    <t>BL-A1.1-3</t>
-  </si>
-  <si>
-    <t>BL-A1.1-4</t>
-  </si>
-  <si>
-    <t>BL-A1.1-5</t>
-  </si>
-  <si>
-    <t>BL-A1.1-6</t>
-  </si>
-  <si>
-    <t>BL-A1.1-7</t>
-  </si>
-  <si>
-    <t>BL-A1.1-8</t>
-  </si>
-  <si>
-    <t>BL-A1.1-9</t>
-  </si>
-  <si>
-    <t>BL-A1.1-10</t>
-  </si>
-  <si>
-    <t>BL-A1.1-11</t>
-  </si>
-  <si>
-    <t>BL-A1.1-12</t>
-  </si>
-  <si>
-    <t>BL-A1.1-13</t>
-  </si>
-  <si>
-    <t>BL-A1.1-14</t>
-  </si>
-  <si>
-    <t>BL-A1.1-15</t>
-  </si>
-  <si>
-    <t>BL-A1.1-16</t>
-  </si>
-  <si>
-    <t>BL-A1.1-17</t>
-  </si>
-  <si>
-    <t>BL-A1.1-18</t>
-  </si>
-  <si>
-    <t>BL-A1.1-19</t>
-  </si>
-  <si>
-    <t>BL-A1.1-20</t>
-  </si>
-  <si>
-    <t>BL-A1.1-21</t>
-  </si>
-  <si>
-    <t>BL-A1.1-22</t>
-  </si>
-  <si>
-    <t>BL-A1.1-23</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>B bw</t>
-  </si>
-  <si>
-    <t>BL-B1.1-0</t>
-  </si>
-  <si>
-    <t>BL-B1.1-1</t>
-  </si>
-  <si>
-    <t>BL-B1.1-2</t>
-  </si>
-  <si>
-    <t>BL-B1.1-3</t>
-  </si>
-  <si>
-    <t>BL-B1.1-4</t>
-  </si>
-  <si>
-    <t>BL-B1.1-5</t>
-  </si>
-  <si>
-    <t>BL-B1.1-6</t>
-  </si>
-  <si>
-    <t>BL-B1.1-7</t>
-  </si>
-  <si>
-    <t>BL-B1.1-8</t>
-  </si>
-  <si>
-    <t>BL-B1.1-9</t>
-  </si>
-  <si>
-    <t>BL-B1.1-10</t>
-  </si>
-  <si>
-    <t>BL-B1.1-11</t>
-  </si>
-  <si>
-    <t>BL-B1.1-12</t>
-  </si>
-  <si>
-    <t>BL-B1.1-13</t>
-  </si>
-  <si>
-    <t>BL-B1.1-14</t>
-  </si>
-  <si>
-    <t>BL-B1.1-15</t>
-  </si>
-  <si>
-    <t>BL-B1.1-16</t>
-  </si>
-  <si>
-    <t>BL-B1.1-17</t>
-  </si>
-  <si>
-    <t>BL-B1.1-18</t>
-  </si>
-  <si>
-    <t>BL-B1.1-19</t>
-  </si>
-  <si>
-    <t>BL-B1.1-20</t>
-  </si>
-  <si>
-    <t>BL-B1.1-21</t>
-  </si>
-  <si>
-    <t>BL-B1.1-22</t>
-  </si>
-  <si>
-    <t>BL-B1.1-23</t>
-  </si>
-  <si>
-    <t>BL-B1.1-24</t>
-  </si>
-  <si>
-    <t>C bw</t>
-  </si>
-  <si>
-    <t>BL-C1.1-0</t>
-  </si>
-  <si>
-    <t>BL-C1.1-1</t>
-  </si>
-  <si>
-    <t>BL-C1.1-2</t>
-  </si>
-  <si>
-    <t>BL-C1.1-3</t>
-  </si>
-  <si>
-    <t>BL-C1.1-4</t>
-  </si>
-  <si>
-    <t>BL-C1.1-5</t>
-  </si>
-  <si>
-    <t>BL-C1.1-6</t>
-  </si>
-  <si>
-    <t>BL-C1.1-7</t>
-  </si>
-  <si>
-    <t>BL-C1.1-8</t>
-  </si>
-  <si>
-    <t>BL-C1.1-9</t>
-  </si>
-  <si>
-    <t>BL-C1.1-10</t>
-  </si>
-  <si>
-    <t>BL-C1.1-11</t>
-  </si>
-  <si>
-    <t>BL-C1.1-12</t>
-  </si>
-  <si>
-    <t>BL-C1.1-13</t>
-  </si>
-  <si>
-    <t>BL-C1.1-14</t>
-  </si>
-  <si>
-    <t>BL-C1.1-15</t>
-  </si>
-  <si>
-    <t>BL-C1.1-16</t>
-  </si>
-  <si>
-    <t>BL-C1.1-17</t>
-  </si>
-  <si>
-    <t>BL-C1.1-18</t>
-  </si>
-  <si>
-    <t>BL-C1.1-19</t>
-  </si>
-  <si>
-    <t>BL-C1.1-20</t>
-  </si>
-  <si>
-    <t>BL-C1.1-21</t>
-  </si>
-  <si>
-    <t>BL-C1.1-22</t>
-  </si>
-  <si>
-    <t>BL-C1.1-23</t>
-  </si>
-  <si>
-    <t>BL-C1.1-24</t>
-  </si>
-  <si>
-    <t>BL-C1.1-25</t>
-  </si>
-  <si>
-    <t>BL-C1.1-26</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>D bw</t>
-  </si>
-  <si>
-    <t>BL-D1.1-0</t>
-  </si>
-  <si>
-    <t>BL-D1.1-1</t>
-  </si>
-  <si>
-    <t>BL-D1.1-2</t>
-  </si>
-  <si>
-    <t>BL-D1.1-3</t>
-  </si>
-  <si>
-    <t>BL-D1.1-4</t>
-  </si>
-  <si>
-    <t>BL-D1.1-5</t>
-  </si>
-  <si>
-    <t>BL-D1.1-6</t>
-  </si>
-  <si>
-    <t>BL-D1.1-7</t>
-  </si>
-  <si>
-    <t>BL-D1.1-8</t>
-  </si>
-  <si>
-    <t>BL-D1.1-9</t>
-  </si>
-  <si>
-    <t>BL-D1.1-10</t>
-  </si>
-  <si>
-    <t>BL-D1.1-11</t>
-  </si>
-  <si>
-    <t>BL-D1.1-12</t>
-  </si>
-  <si>
-    <t>BL-D1.1-13</t>
-  </si>
-  <si>
-    <t>BL-D1.1-14</t>
-  </si>
-  <si>
-    <t>BL-D1.1-15</t>
-  </si>
-  <si>
-    <t>BL-D1.1-16</t>
-  </si>
-  <si>
-    <t>BL-D1.1-17</t>
-  </si>
-  <si>
-    <t>BL-D1.1-18</t>
-  </si>
-  <si>
-    <t>BL-D1.1-19</t>
-  </si>
-  <si>
-    <t>BL-D1.1-20</t>
-  </si>
-  <si>
-    <t>BL-D1.1-21</t>
-  </si>
-  <si>
-    <t>BL-D1.1-22</t>
-  </si>
-  <si>
-    <t>BL-D1.1-23</t>
-  </si>
-  <si>
-    <t>BL-D1.1-24</t>
-  </si>
-  <si>
-    <t>BL-D1.1-25</t>
-  </si>
-  <si>
-    <t>BL-D1.1-26</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -382,6 +61,330 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BL-A-sw1</t>
+  </si>
+  <si>
+    <t>BL-D-sw1</t>
+  </si>
+  <si>
+    <t>BL-C-sw1</t>
+  </si>
+  <si>
+    <t>BL-B-sw1</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-0</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-1</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-2</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-3</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-4</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-5</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-6</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-7</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-8</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-9</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-10</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-11</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-12</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-13</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-14</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-15</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-16</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-17</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-18</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-19</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-20</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-21</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-22</t>
+  </si>
+  <si>
+    <t>BL-A1.1-pw-23</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-0</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-1</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-2</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-3</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-4</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-5</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-6</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-7</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-8</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-9</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-10</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-11</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-12</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-13</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-14</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-15</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-16</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-17</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-18</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-19</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-20</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-21</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-22</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-23</t>
+  </si>
+  <si>
+    <t>BL-B1.1-pw-24</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-0</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-1</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-2</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-3</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-4</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-5</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-6</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-7</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-8</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-9</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-10</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-11</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-12</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-13</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-14</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-15</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-16</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-17</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-18</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-19</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-20</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-21</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-22</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-23</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-24</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-25</t>
+  </si>
+  <si>
+    <t>BL-C1.1-pw-26</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-0</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-1</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-2</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-3</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-4</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-5</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-6</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-7</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-8</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-9</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-10</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-11</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-12</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-13</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-14</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-15</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-16</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-17</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-18</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-19</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-20</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-21</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-22</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-23</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-24</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-25</t>
+  </si>
+  <si>
+    <t>BL-D1.1-pw-26</t>
   </si>
 </sst>
 </file>
@@ -714,15 +717,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H118" sqref="G118:H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -731,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -745,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -765,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -785,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -805,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -825,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -845,7 +848,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -865,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -885,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -905,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -925,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -945,7 +948,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -965,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -985,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>14</v>
@@ -1005,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1025,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>18</v>
@@ -1045,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -1065,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>22</v>
@@ -1085,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>24</v>
@@ -1105,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>26</v>
@@ -1125,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>28</v>
@@ -1145,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>30</v>
@@ -1165,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>32</v>
@@ -1185,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <v>34</v>
@@ -1205,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C25">
         <v>36</v>
@@ -1225,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>38</v>
@@ -1242,10 +1245,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1262,10 +1265,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1282,10 +1285,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1302,10 +1305,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1322,10 +1325,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1342,10 +1345,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -1362,10 +1365,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -1382,10 +1385,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C34">
         <v>7</v>
@@ -1402,10 +1405,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -1422,10 +1425,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -1442,10 +1445,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1462,10 +1465,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C38">
         <v>12</v>
@@ -1482,10 +1485,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C39">
         <v>14</v>
@@ -1502,10 +1505,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C40">
         <v>16</v>
@@ -1522,10 +1525,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C41">
         <v>18</v>
@@ -1542,10 +1545,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C42">
         <v>20</v>
@@ -1562,10 +1565,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C43">
         <v>22</v>
@@ -1582,10 +1585,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C44">
         <v>24</v>
@@ -1602,10 +1605,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>26</v>
@@ -1622,10 +1625,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C46">
         <v>28</v>
@@ -1642,10 +1645,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C47">
         <v>30</v>
@@ -1662,10 +1665,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C48">
         <v>32</v>
@@ -1682,10 +1685,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C49">
         <v>34</v>
@@ -1702,10 +1705,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C50">
         <v>36</v>
@@ -1722,10 +1725,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C51">
         <v>38</v>
@@ -1742,10 +1745,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C52">
         <v>40</v>
@@ -1762,10 +1765,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1782,10 +1785,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1802,10 +1805,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -1822,10 +1825,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1842,10 +1845,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -1862,10 +1865,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -1882,10 +1885,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -1902,10 +1905,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>7</v>
@@ -1922,10 +1925,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -1942,10 +1945,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C62">
         <v>9</v>
@@ -1962,10 +1965,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C63">
         <v>10</v>
@@ -1982,10 +1985,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C64">
         <v>12</v>
@@ -2002,10 +2005,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C65">
         <v>14</v>
@@ -2022,10 +2025,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C66">
         <v>16</v>
@@ -2042,10 +2045,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C67">
         <v>18</v>
@@ -2057,10 +2060,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C68">
         <v>20</v>
@@ -2077,10 +2080,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C69">
         <v>22</v>
@@ -2097,10 +2100,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C70">
         <v>24</v>
@@ -2117,10 +2120,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C71">
         <v>26</v>
@@ -2137,10 +2140,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C72">
         <v>28</v>
@@ -2157,10 +2160,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C73">
         <v>30</v>
@@ -2177,10 +2180,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C74">
         <v>32</v>
@@ -2197,10 +2200,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C75">
         <v>34</v>
@@ -2217,10 +2220,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C76">
         <v>36</v>
@@ -2237,10 +2240,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C77">
         <v>38</v>
@@ -2257,10 +2260,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C78">
         <v>40</v>
@@ -2277,10 +2280,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C79">
         <v>42</v>
@@ -2297,10 +2300,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C80">
         <v>44</v>
@@ -2317,10 +2320,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2337,10 +2340,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2357,10 +2360,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -2377,10 +2380,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2397,10 +2400,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -2417,10 +2420,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C86">
         <v>5</v>
@@ -2437,10 +2440,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C87">
         <v>6</v>
@@ -2457,10 +2460,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C88">
         <v>7</v>
@@ -2477,10 +2480,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C89">
         <v>8</v>
@@ -2497,10 +2500,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C90">
         <v>9</v>
@@ -2517,10 +2520,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C91">
         <v>10</v>
@@ -2537,10 +2540,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C92">
         <v>12</v>
@@ -2557,10 +2560,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C93">
         <v>14</v>
@@ -2577,10 +2580,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C94">
         <v>16</v>
@@ -2597,10 +2600,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C95">
         <v>18</v>
@@ -2617,10 +2620,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C96">
         <v>20</v>
@@ -2637,10 +2640,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C97">
         <v>22</v>
@@ -2657,10 +2660,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C98">
         <v>24</v>
@@ -2677,10 +2680,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C99">
         <v>26</v>
@@ -2697,10 +2700,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C100">
         <v>28</v>
@@ -2717,10 +2720,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C101">
         <v>30</v>
@@ -2737,10 +2740,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C102">
         <v>32</v>
@@ -2757,10 +2760,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C103">
         <v>34</v>
@@ -2777,10 +2780,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C104">
         <v>36</v>
@@ -2797,10 +2800,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C105">
         <v>38</v>
@@ -2817,10 +2820,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C106">
         <v>40</v>
@@ -2837,10 +2840,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C107">
         <v>42</v>
@@ -2857,10 +2860,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C108">
         <v>44</v>

</xml_diff>

<commit_message>
created nice plots for IC porwater profiles.
</commit_message>
<xml_diff>
--- a/index/data/pw_P_photometric.xlsx
+++ b/index/data/pw_P_photometric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD42BCF-164D-4237-96FB-AD20694F7652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FA3400-F0B1-4F4F-877D-35D11FCE79BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Fetot</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>BL-D1.1-pw-26</t>
+  </si>
+  <si>
+    <t>P_phot</t>
   </si>
 </sst>
 </file>
@@ -717,15 +717,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H118" sqref="G118:H122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -734,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -748,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -828,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -848,7 +848,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -908,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -928,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -948,7 +948,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -968,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>14</v>
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>18</v>
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -1068,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>22</v>
@@ -1088,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>24</v>
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>26</v>
@@ -1128,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>28</v>
@@ -1148,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>30</v>
@@ -1168,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>32</v>
@@ -1188,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>34</v>
@@ -1208,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>36</v>
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>38</v>
@@ -1248,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1268,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1288,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1308,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1328,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1348,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -1368,7 +1368,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>7</v>
@@ -1408,7 +1408,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -1428,7 +1428,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -1448,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1468,7 +1468,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38">
         <v>12</v>
@@ -1488,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39">
         <v>14</v>
@@ -1508,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40">
         <v>16</v>
@@ -1528,7 +1528,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41">
         <v>18</v>
@@ -1548,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42">
         <v>20</v>
@@ -1568,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43">
         <v>22</v>
@@ -1588,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44">
         <v>24</v>
@@ -1608,7 +1608,7 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45">
         <v>26</v>
@@ -1628,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>28</v>
@@ -1648,7 +1648,7 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47">
         <v>30</v>
@@ -1668,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48">
         <v>32</v>
@@ -1688,7 +1688,7 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49">
         <v>34</v>
@@ -1708,7 +1708,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50">
         <v>36</v>
@@ -1728,7 +1728,7 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51">
         <v>38</v>
@@ -1748,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52">
         <v>40</v>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1805,10 +1805,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1845,10 +1845,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -1885,10 +1885,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60">
         <v>7</v>
@@ -1925,10 +1925,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -1945,10 +1945,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>9</v>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>10</v>
@@ -1985,10 +1985,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>12</v>
@@ -2005,10 +2005,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65">
         <v>14</v>
@@ -2025,10 +2025,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66">
         <v>16</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67">
         <v>18</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68">
         <v>20</v>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>22</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70">
         <v>24</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71">
         <v>26</v>
@@ -2140,10 +2140,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72">
         <v>28</v>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73">
         <v>30</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74">
         <v>32</v>
@@ -2200,10 +2200,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75">
         <v>34</v>
@@ -2220,10 +2220,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76">
         <v>36</v>
@@ -2240,10 +2240,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77">
         <v>38</v>
@@ -2260,10 +2260,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78">
         <v>40</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79">
         <v>42</v>
@@ -2300,10 +2300,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80">
         <v>44</v>
@@ -2323,7 +2323,7 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2343,7 +2343,7 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2363,7 +2363,7 @@
         <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -2383,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2403,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -2423,7 +2423,7 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86">
         <v>5</v>
@@ -2443,7 +2443,7 @@
         <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87">
         <v>6</v>
@@ -2463,7 +2463,7 @@
         <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88">
         <v>7</v>
@@ -2483,7 +2483,7 @@
         <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C89">
         <v>8</v>
@@ -2503,7 +2503,7 @@
         <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90">
         <v>9</v>
@@ -2523,7 +2523,7 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91">
         <v>10</v>
@@ -2543,7 +2543,7 @@
         <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92">
         <v>12</v>
@@ -2563,7 +2563,7 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93">
         <v>14</v>
@@ -2583,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C94">
         <v>16</v>
@@ -2603,7 +2603,7 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C95">
         <v>18</v>
@@ -2623,7 +2623,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C96">
         <v>20</v>
@@ -2643,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C97">
         <v>22</v>
@@ -2663,7 +2663,7 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C98">
         <v>24</v>
@@ -2683,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99">
         <v>26</v>
@@ -2703,7 +2703,7 @@
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C100">
         <v>28</v>
@@ -2723,7 +2723,7 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C101">
         <v>30</v>
@@ -2743,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C102">
         <v>32</v>
@@ -2763,7 +2763,7 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C103">
         <v>34</v>
@@ -2783,7 +2783,7 @@
         <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C104">
         <v>36</v>
@@ -2803,7 +2803,7 @@
         <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C105">
         <v>38</v>
@@ -2823,7 +2823,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C106">
         <v>40</v>
@@ -2843,7 +2843,7 @@
         <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C107">
         <v>42</v>
@@ -2863,7 +2863,7 @@
         <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C108">
         <v>44</v>

</xml_diff>